<commit_message>
commit species fix to only process the rows that discuss soil
</commit_message>
<xml_diff>
--- a/chatgpt_vekstmedium_2023.11.12/Data/2_processed_data/chatgpt_vksmedium_yes_no.xlsx
+++ b/chatgpt_vekstmedium_2023.11.12/Data/2_processed_data/chatgpt_vksmedium_yes_no.xlsx
@@ -440,7 +440,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Comparative analysis of grape cultivation in Tamil Nadu found that using 'Dog Ridge' rootstock for 'Muscat Hamburg' grapes led to better growth, yield, and nutrient content compared to self-rooted cuttings.</t>
+          <t>Growth and yield of 'Muscat Hamburg' grape was compared when grafted on 'Dog Ridge' rootstock and self-rooted cuttings in Tamil Nadu, India. Grafted vines showed better results.</t>
         </is>
       </c>
     </row>
@@ -460,7 +460,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Silicon preparations were tested on pine and oak seedlings and found to increase growth, photosynthetic efficiency, and biomass, particularly at a concentration of 2%.</t>
+          <t>Silicon preparations can promote growth in forest seedlings, increasing biomass and improving nutritional value. Spraying with a 2% concentration is most effective, particularly for oak seedlings.</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>The study examined the effects of soil media mixtures with phosphogypsum on young pine seedlings, finding no harmful effects. Further testing on heavy metals and long-term effects is needed.</t>
+          <t>This study investigated the effects of different soil media mixtures containing phosphogypsum on the growth of young pine seedlings. The mixtures did not have harmful effects, but longer-term observations are needed. Lower dosages appear to be more promising and cost-effective. Further testing is recommended for heavy metals and microbiome changes.</t>
         </is>
       </c>
     </row>
@@ -515,7 +515,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>This study explores the growth-survival trade-off in non-phanerophyte species used in dune restoration. Findings suggest targeting foredune species for cost-effective restoration actions based on their low survival rates and reproductive effort.</t>
+          <t>This study investigates the growth-survival trade-offs in non-phanerophyte species used in a coastal dune restoration project. The results suggest that plant species of foredune communities have higher growth but lower survival rates, providing insights for cost-effective ecosystem restoration actions.</t>
         </is>
       </c>
     </row>
@@ -535,7 +535,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>A study on eelgrass restoration in Sweden found rapid colonization of invertebrates in all plots, regardless of patch size. Smaller patches can be as effective as continuous patches in promoting biodiversity. Variability between years emphasizes the need for monitoring.</t>
+          <t>A study found that the colonization of fauna in eelgrass restoration plots was rapid and similar regardless of patch size, suggesting smaller patches can be as effective for promoting biodiversity.</t>
         </is>
       </c>
     </row>
@@ -550,12 +550,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>The study investigates the relationship between seed production and pine regeneration using nutcracker birds as mediators. Results show that the abundance of seedlings depends on the number of birds and seeds.</t>
+          <t>No</t>
         </is>
       </c>
     </row>

</xml_diff>